<commit_message>
Large Dataset files cleanup
</commit_message>
<xml_diff>
--- a/Large Dataset/blender/data/blender results.xlsx
+++ b/Large Dataset/blender/data/blender results.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carson/Desktop/Pioneer Paper/ML models/blender/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carson/Desktop/Pioneer Paper/CPU-Features-and-Benchmarks-using-Machine-Learning/Large Dataset/blender/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87623364-086C-7C4A-A871-A02C35A9820B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBB31388-21C9-9C4E-87AB-EC5EAAAD3FAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33600" yWindow="-600" windowWidth="38400" windowHeight="21600" xr2:uid="{08D759DD-F865-0C4C-B258-11A8D1ABDA2D}"/>
+    <workbookView xWindow="33600" yWindow="-100" windowWidth="38400" windowHeight="21100" xr2:uid="{08D759DD-F865-0C4C-B258-11A8D1ABDA2D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="19">
   <si>
     <t>Trial</t>
   </si>
@@ -101,7 +101,7 @@
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0000000"/>
-    <numFmt numFmtId="169" formatCode="0.0000"/>
+    <numFmt numFmtId="166" formatCode="0.0000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -136,7 +136,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -439,28 +439,28 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>2.0270341000000001E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.5504097000000003E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.1601952000000003E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.7298649000000001E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.12797661499999996</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.0958634E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.74677429100000003</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>9.6154199999999995E-3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1457,8 +1457,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5F1C417-443F-BB40-8A17-99E410E545BB}">
   <dimension ref="A1:J80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="220" workbookViewId="0">
-      <selection activeCell="E62" sqref="E62"/>
+    <sheetView tabSelected="1" topLeftCell="A65" zoomScale="220" workbookViewId="0">
+      <selection activeCell="A75" sqref="A75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2289,324 +2289,108 @@
       <c r="H58" s="3"/>
       <c r="I58" s="3"/>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A68" t="s">
-        <v>0</v>
-      </c>
-      <c r="B68" t="s">
-        <v>5</v>
-      </c>
-      <c r="C68" t="s">
-        <v>6</v>
-      </c>
-      <c r="D68" t="s">
-        <v>7</v>
-      </c>
-      <c r="E68" t="s">
-        <v>8</v>
-      </c>
-      <c r="F68" t="s">
-        <v>9</v>
-      </c>
-      <c r="G68" t="s">
-        <v>10</v>
-      </c>
-      <c r="H68" t="s">
-        <v>11</v>
-      </c>
-      <c r="I68" t="s">
-        <v>12</v>
-      </c>
-    </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A69">
-        <v>1</v>
-      </c>
-      <c r="B69" s="1">
-        <v>4.4219920000000003E-2</v>
-      </c>
-      <c r="C69" s="1">
-        <v>6.3501399999999998E-3</v>
-      </c>
-      <c r="D69" s="1">
-        <v>3.5068950000000002E-2</v>
-      </c>
-      <c r="E69" s="1">
-        <v>2.6701820000000001E-2</v>
-      </c>
-      <c r="F69" s="1">
-        <v>0.13806495999999999</v>
-      </c>
-      <c r="G69" s="1">
-        <v>8.7244899999999997E-3</v>
-      </c>
-      <c r="H69" s="1">
-        <v>0.73700180000000004</v>
-      </c>
-      <c r="I69" s="1">
-        <v>3.86792E-3</v>
-      </c>
+      <c r="B69" s="1"/>
+      <c r="C69" s="1"/>
+      <c r="D69" s="1"/>
+      <c r="E69" s="1"/>
+      <c r="F69" s="1"/>
+      <c r="G69" s="1"/>
+      <c r="H69" s="1"/>
+      <c r="I69" s="1"/>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A70">
-        <v>2</v>
-      </c>
-      <c r="B70" s="1">
-        <v>3.12692E-3</v>
-      </c>
-      <c r="C70" s="1">
-        <v>4.7026030000000003E-2</v>
-      </c>
-      <c r="D70" s="1">
-        <v>2.263362E-2</v>
-      </c>
-      <c r="E70" s="1">
-        <v>4.0574190000000003E-2</v>
-      </c>
-      <c r="F70" s="1">
-        <v>0.13676737</v>
-      </c>
-      <c r="G70" s="1">
-        <v>3.8503500000000002E-3</v>
-      </c>
-      <c r="H70" s="1">
-        <v>0.74185827000000004</v>
-      </c>
-      <c r="I70" s="1">
-        <v>4.1632600000000002E-3</v>
-      </c>
+      <c r="B70" s="1"/>
+      <c r="C70" s="1"/>
+      <c r="D70" s="1"/>
+      <c r="E70" s="1"/>
+      <c r="F70" s="1"/>
+      <c r="G70" s="1"/>
+      <c r="H70" s="1"/>
+      <c r="I70" s="1"/>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A71">
-        <v>3</v>
-      </c>
-      <c r="B71" s="1">
-        <v>2.8560459999999999E-2</v>
-      </c>
-      <c r="C71" s="1">
-        <v>1.110445E-2</v>
-      </c>
-      <c r="D71" s="1">
-        <v>3.29022E-2</v>
-      </c>
-      <c r="E71" s="1">
-        <v>2.6623290000000001E-2</v>
-      </c>
-      <c r="F71" s="1">
-        <v>0.13091438</v>
-      </c>
-      <c r="G71" s="1">
-        <v>3.73128E-3</v>
-      </c>
-      <c r="H71" s="1">
-        <v>0.76206348999999995</v>
-      </c>
-      <c r="I71" s="1">
-        <v>4.1004500000000003E-3</v>
-      </c>
+      <c r="B71" s="1"/>
+      <c r="C71" s="1"/>
+      <c r="D71" s="1"/>
+      <c r="E71" s="1"/>
+      <c r="F71" s="1"/>
+      <c r="G71" s="1"/>
+      <c r="H71" s="1"/>
+      <c r="I71" s="1"/>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A72">
-        <v>4</v>
-      </c>
-      <c r="B72" s="1">
-        <v>2.397148E-2</v>
-      </c>
-      <c r="C72" s="1">
-        <v>3.0023879999999999E-2</v>
-      </c>
-      <c r="D72" s="1">
-        <v>3.4541969999999998E-2</v>
-      </c>
-      <c r="E72" s="1">
-        <v>2.2666760000000001E-2</v>
-      </c>
-      <c r="F72" s="1">
-        <v>0.11073653</v>
-      </c>
-      <c r="G72" s="1">
-        <v>7.1455700000000004E-3</v>
-      </c>
-      <c r="H72" s="1">
-        <v>0.76374498000000002</v>
-      </c>
-      <c r="I72" s="1">
-        <v>7.1688400000000001E-3</v>
-      </c>
+      <c r="B72" s="1"/>
+      <c r="C72" s="1"/>
+      <c r="D72" s="1"/>
+      <c r="E72" s="1"/>
+      <c r="F72" s="1"/>
+      <c r="G72" s="1"/>
+      <c r="H72" s="1"/>
+      <c r="I72" s="1"/>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A73">
-        <v>5</v>
-      </c>
-      <c r="B73" s="1">
-        <v>1.1221760000000001E-2</v>
-      </c>
-      <c r="C73" s="1">
-        <v>3.2073280000000003E-2</v>
-      </c>
-      <c r="D73" s="1">
-        <v>2.645629E-2</v>
-      </c>
-      <c r="E73" s="1">
-        <v>3.3363080000000003E-2</v>
-      </c>
-      <c r="F73" s="1">
-        <v>0.10426782</v>
-      </c>
-      <c r="G73" s="1">
-        <v>2.2837500000000002E-3</v>
-      </c>
-      <c r="H73" s="1">
-        <v>0.77571431999999996</v>
-      </c>
-      <c r="I73" s="1">
-        <v>1.4619699999999999E-2</v>
-      </c>
+      <c r="B73" s="1"/>
+      <c r="C73" s="1"/>
+      <c r="D73" s="1"/>
+      <c r="E73" s="1"/>
+      <c r="F73" s="1"/>
+      <c r="G73" s="1"/>
+      <c r="H73" s="1"/>
+      <c r="I73" s="1"/>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A74">
-        <v>6</v>
-      </c>
-      <c r="B74" s="1">
-        <v>2.422467E-2</v>
-      </c>
-      <c r="C74" s="1">
-        <v>2.4528319999999999E-2</v>
-      </c>
-      <c r="D74" s="1">
-        <v>3.3234029999999998E-2</v>
-      </c>
-      <c r="E74" s="1">
-        <v>2.3605709999999998E-2</v>
-      </c>
-      <c r="F74" s="1">
-        <v>0.12421875</v>
-      </c>
-      <c r="G74" s="1">
-        <v>8.5184800000000001E-3</v>
-      </c>
-      <c r="H74" s="1">
-        <v>0.75504848999999996</v>
-      </c>
-      <c r="I74" s="1">
-        <v>6.6215400000000004E-3</v>
-      </c>
+      <c r="B74" s="1"/>
+      <c r="C74" s="1"/>
+      <c r="D74" s="1"/>
+      <c r="E74" s="1"/>
+      <c r="F74" s="1"/>
+      <c r="G74" s="1"/>
+      <c r="H74" s="1"/>
+      <c r="I74" s="1"/>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A75">
-        <v>7</v>
-      </c>
-      <c r="B75" s="1">
-        <v>1.08658E-3</v>
-      </c>
-      <c r="C75" s="1">
-        <v>5.253323E-2</v>
-      </c>
-      <c r="D75" s="1">
-        <v>3.1317119999999997E-2</v>
-      </c>
-      <c r="E75" s="1">
-        <v>2.83127E-2</v>
-      </c>
-      <c r="F75" s="1">
-        <v>0.13544106</v>
-      </c>
-      <c r="G75" s="1">
-        <v>6.0244520000000003E-2</v>
-      </c>
-      <c r="H75" s="1">
-        <v>0.68712523000000003</v>
-      </c>
-      <c r="I75" s="1">
-        <v>3.9395599999999999E-3</v>
-      </c>
+      <c r="B75" s="1"/>
+      <c r="C75" s="1"/>
+      <c r="D75" s="1"/>
+      <c r="E75" s="1"/>
+      <c r="F75" s="1"/>
+      <c r="G75" s="1"/>
+      <c r="H75" s="1"/>
+      <c r="I75" s="1"/>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A76">
-        <v>8</v>
-      </c>
-      <c r="B76" s="1">
-        <v>1.4379799999999999E-3</v>
-      </c>
-      <c r="C76" s="1">
-        <v>3.0079229999999998E-2</v>
-      </c>
-      <c r="D76" s="1">
-        <v>3.4340799999999998E-2</v>
-      </c>
-      <c r="E76" s="1">
-        <v>2.1592210000000001E-2</v>
-      </c>
-      <c r="F76" s="1">
-        <v>0.12714713999999999</v>
-      </c>
-      <c r="G76" s="1">
-        <v>6.5163299999999999E-3</v>
-      </c>
-      <c r="H76" s="1">
-        <v>0.75099406000000002</v>
-      </c>
-      <c r="I76" s="1">
-        <v>2.7892239999999999E-2</v>
-      </c>
+      <c r="B76" s="1"/>
+      <c r="C76" s="1"/>
+      <c r="D76" s="1"/>
+      <c r="E76" s="1"/>
+      <c r="F76" s="1"/>
+      <c r="G76" s="1"/>
+      <c r="H76" s="1"/>
+      <c r="I76" s="1"/>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A77">
-        <v>9</v>
-      </c>
-      <c r="B77" s="1">
-        <v>3.6379849999999998E-2</v>
-      </c>
-      <c r="C77" s="1">
-        <v>6.3421700000000003E-3</v>
-      </c>
-      <c r="D77" s="1">
-        <v>3.8060549999999999E-2</v>
-      </c>
-      <c r="E77" s="1">
-        <v>2.8697730000000001E-2</v>
-      </c>
-      <c r="F77" s="1">
-        <v>0.14839689</v>
-      </c>
-      <c r="G77" s="1">
-        <v>3.3122899999999999E-3</v>
-      </c>
-      <c r="H77" s="1">
-        <v>0.73534838000000002</v>
-      </c>
-      <c r="I77" s="1">
-        <v>3.4621299999999999E-3</v>
-      </c>
+      <c r="B77" s="1"/>
+      <c r="C77" s="1"/>
+      <c r="D77" s="1"/>
+      <c r="E77" s="1"/>
+      <c r="F77" s="1"/>
+      <c r="G77" s="1"/>
+      <c r="H77" s="1"/>
+      <c r="I77" s="1"/>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A78">
-        <v>10</v>
-      </c>
-      <c r="B78" s="1">
-        <v>2.8473789999999999E-2</v>
-      </c>
-      <c r="C78" s="1">
-        <v>1.4980240000000001E-2</v>
-      </c>
-      <c r="D78" s="1">
-        <v>2.7463990000000001E-2</v>
-      </c>
-      <c r="E78" s="1">
-        <v>2.0848999999999999E-2</v>
-      </c>
-      <c r="F78" s="1">
-        <v>0.12381125</v>
-      </c>
-      <c r="G78" s="1">
-        <v>5.2592799999999999E-3</v>
-      </c>
-      <c r="H78" s="1">
-        <v>0.75884388999999997</v>
-      </c>
-      <c r="I78" s="1">
-        <v>2.0318559999999999E-2</v>
-      </c>
+      <c r="A78" t="s">
+        <v>14</v>
+      </c>
+      <c r="B78" s="1"/>
+      <c r="C78" s="1"/>
+      <c r="D78" s="1"/>
+      <c r="E78" s="1"/>
+      <c r="F78" s="1"/>
+      <c r="G78" s="1"/>
+      <c r="H78" s="1"/>
+      <c r="I78" s="1"/>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B79" s="2" t="s">
@@ -2638,37 +2422,37 @@
       <c r="A80" t="s">
         <v>4</v>
       </c>
-      <c r="B80" s="1">
+      <c r="B80" s="1" t="e">
         <f>AVERAGE(B69:B78)</f>
-        <v>2.0270341000000001E-2</v>
-      </c>
-      <c r="C80" s="1">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C80" s="1" t="e">
         <f t="shared" ref="C80:I80" si="1">AVERAGE(C69:C78)</f>
-        <v>2.5504097000000003E-2</v>
-      </c>
-      <c r="D80" s="1">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D80" s="1" t="e">
         <f t="shared" si="1"/>
-        <v>3.1601952000000003E-2</v>
-      </c>
-      <c r="E80" s="1">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E80" s="1" t="e">
         <f t="shared" si="1"/>
-        <v>2.7298649000000001E-2</v>
-      </c>
-      <c r="F80" s="1">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F80" s="1" t="e">
         <f t="shared" si="1"/>
-        <v>0.12797661499999996</v>
-      </c>
-      <c r="G80" s="1">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G80" s="1" t="e">
         <f t="shared" si="1"/>
-        <v>1.0958634E-2</v>
-      </c>
-      <c r="H80" s="1">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H80" s="1" t="e">
         <f t="shared" si="1"/>
-        <v>0.74677429100000003</v>
-      </c>
-      <c r="I80" s="1">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I80" s="1" t="e">
         <f t="shared" si="1"/>
-        <v>9.6154199999999995E-3</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
   </sheetData>

</xml_diff>